<commit_message>
Done with remove duplicates
</commit_message>
<xml_diff>
--- a/backend/demo_files/dummy_excel.xlsx
+++ b/backend/demo_files/dummy_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth\Desktop\Clients data\Neha DS\code\ds-v1\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth\Desktop\Clients data\Neha DS\code\dsv3\backend\demo_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE04549E-8D0C-42F8-A809-666E579A1842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20E1766-9129-4C67-954F-9961EE0641A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="615" windowWidth="27495" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -567,13 +567,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:E14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -607,7 +609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -624,7 +626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -641,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -658,7 +660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -675,7 +677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -692,7 +694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -709,7 +711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -726,7 +728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -743,7 +745,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -760,7 +762,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -777,7 +779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -792,12 +794,29 @@
       </c>
       <c r="E13" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14">
+        <v>5.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F15" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F13 A15:F15 F14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>